<commit_message>
update data jabar dalam angka.
</commit_message>
<xml_diff>
--- a/Jabar/Jabar.xlsx
+++ b/Jabar/Jabar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\System Dynamics\Github\system_dynamics_reference\Jabar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0867787A-2792-4F64-91E0-88B89663D54A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E5E6B85-86C8-49A2-A65B-0C588B5AD176}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="671" xr2:uid="{02F994C9-703D-4073-B38E-810FA24E22F7}"/>
+    <workbookView xWindow="5100" yWindow="1695" windowWidth="21600" windowHeight="11505" tabRatio="671" firstSheet="12" activeTab="14" xr2:uid="{02F994C9-703D-4073-B38E-810FA24E22F7}"/>
   </bookViews>
   <sheets>
     <sheet name="data jabar" sheetId="3" r:id="rId1"/>
@@ -26,6 +26,8 @@
     <sheet name="Energi-Industri" sheetId="6" r:id="rId11"/>
     <sheet name="Energi-Komersial" sheetId="7" r:id="rId12"/>
     <sheet name="Energi-Lainnya" sheetId="8" r:id="rId13"/>
+    <sheet name="Industri, 2015" sheetId="15" r:id="rId14"/>
+    <sheet name="Jabar dalam Angka" sheetId="16" r:id="rId15"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -78,8 +80,189 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>wizard</author>
+  </authors>
+  <commentList>
+    <comment ref="Z10" authorId="0" shapeId="0" xr:uid="{30A92EBF-F60B-40EE-8C6E-E0BDAB9B1AF1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>wizard:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+data asli dalam milyar rupiah</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Y11" authorId="0" shapeId="0" xr:uid="{1CEDF3FA-2F35-4F64-B09E-DA3D3A323F35}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>wizard:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+data asli dalam milyar rupiah
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Z11" authorId="0" shapeId="0" xr:uid="{13C1DC58-7035-4D85-A36C-7565D1522490}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>wizard:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+data asli dalam milyar rupiah</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Y12" authorId="0" shapeId="0" xr:uid="{35F2E029-49D2-438D-9064-F718DF15271D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>wizard:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+data asli dalam milyar rupiah
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Z12" authorId="0" shapeId="0" xr:uid="{B628F096-004F-4A82-8CDB-B4C2420ED066}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>wizard:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+data asli dalam milyar rupiah
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Y13" authorId="0" shapeId="0" xr:uid="{B397A8EA-AF5F-47E9-86DD-DBF34E660E72}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>wizard:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+data asli dalam milyar rupiah</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Z13" authorId="0" shapeId="0" xr:uid="{6304CA0D-A000-457E-AEE7-F25075542A70}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>wizard:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+data asli dalam milyar rupiah</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="178">
   <si>
     <t>Kabupaten/Regency</t>
   </si>
@@ -433,6 +616,186 @@
   </si>
   <si>
     <t>static gdp per capita growth[jabar]</t>
+  </si>
+  <si>
+    <t>Golongan Industri</t>
+  </si>
+  <si>
+    <t>Perusahaan</t>
+  </si>
+  <si>
+    <t>Employment</t>
+  </si>
+  <si>
+    <t>Industri Makanan</t>
+  </si>
+  <si>
+    <t>Industri Minuman</t>
+  </si>
+  <si>
+    <t>Industri Pengolahan Tembakau</t>
+  </si>
+  <si>
+    <t>Industri Pakaian Jadi</t>
+  </si>
+  <si>
+    <t>Industri Kulit, Barang dari Kulit, dan Alas Kaki</t>
+  </si>
+  <si>
+    <t>Industri Tekstil</t>
+  </si>
+  <si>
+    <t>Industri Kayu, Barang dari Kayu (non Furnitur), dan Barang Anyaman dari Rotan, Bambu, dsj.</t>
+  </si>
+  <si>
+    <t>Industri Kertas, Barang dari Kertas, dsj.</t>
+  </si>
+  <si>
+    <t>Industri Percetakan</t>
+  </si>
+  <si>
+    <t>Industri Produk dari batubara, Pengilangan Minyak Bumi</t>
+  </si>
+  <si>
+    <t>Industri Kimia dan Barang dari Bahan Kimia</t>
+  </si>
+  <si>
+    <t>Industri Karet, Barang dari Karet dan Plastik</t>
+  </si>
+  <si>
+    <t>Industri Farmasi, Produk Obat Kimia, dan Obat Traditional</t>
+  </si>
+  <si>
+    <t>Industri Barang Galian non Logam</t>
+  </si>
+  <si>
+    <t>Industri Logam Dasar</t>
+  </si>
+  <si>
+    <t>Industri Barang Logam Bukan Mesin</t>
+  </si>
+  <si>
+    <t>Industri Komputer, Barang Elektronik dan Optik</t>
+  </si>
+  <si>
+    <t>Industri Peralatan Listrik</t>
+  </si>
+  <si>
+    <t>Industri Mesin dan Peralatan</t>
+  </si>
+  <si>
+    <t>Industri Alat Angkutan Lainnya</t>
+  </si>
+  <si>
+    <t>Industri Furnitur</t>
+  </si>
+  <si>
+    <t>Industri Pengolahan Lainnya</t>
+  </si>
+  <si>
+    <t>Jasa Reparasi dan Pemasangan Mesin dan Peralatan</t>
+  </si>
+  <si>
+    <t>Industri Kendaraan Bermotor, Trailer, dan Semi Trailer</t>
+  </si>
+  <si>
+    <t>Biaya Input/Input Cost</t>
+  </si>
+  <si>
+    <t>Nilai Output Kotor / Value of Gross Output</t>
+  </si>
+  <si>
+    <t>Nilai Tambah (Harga Pasar)/Value Added at Market Prices</t>
+  </si>
+  <si>
+    <t>Bahan Baku / Raw Materials</t>
+  </si>
+  <si>
+    <t>Bahan Bakar dan Pelumas / Fuel and Lubricants</t>
+  </si>
+  <si>
+    <t>Listrik / Electricity</t>
+  </si>
+  <si>
+    <t>Sewa Gedung, Mesin, Alat-Alat</t>
+  </si>
+  <si>
+    <t>Jasa Lainnya</t>
+  </si>
+  <si>
+    <t>Populasi</t>
+  </si>
+  <si>
+    <t>Daya Terpasang (KW)</t>
+  </si>
+  <si>
+    <t>Produksi Listrik (KWh)</t>
+  </si>
+  <si>
+    <t>Listrik Terjual (KWh)</t>
+  </si>
+  <si>
+    <t>Dipakai Sendiri (KWh)</t>
+  </si>
+  <si>
+    <t>Susut/Hilang (KWh)</t>
+  </si>
+  <si>
+    <t>Sedan</t>
+  </si>
+  <si>
+    <t>Pribadi</t>
+  </si>
+  <si>
+    <t>Umum</t>
+  </si>
+  <si>
+    <t>Sedan, Jeep, Minibus</t>
+  </si>
+  <si>
+    <t>Bus dan sejenisnya</t>
+  </si>
+  <si>
+    <t>Truk/ Pickup</t>
+  </si>
+  <si>
+    <t>Alat Berat</t>
+  </si>
+  <si>
+    <t>Sepeda Motor</t>
+  </si>
+  <si>
+    <t>Jeep</t>
+  </si>
+  <si>
+    <t>Minibus dan sejenisnya</t>
+  </si>
+  <si>
+    <t>Industri</t>
+  </si>
+  <si>
+    <t>Sektor</t>
+  </si>
+  <si>
+    <t>Nilai Investasi</t>
+  </si>
+  <si>
+    <t>Dalam Negeri</t>
+  </si>
+  <si>
+    <t>Luar Negeri</t>
+  </si>
+  <si>
+    <t>PDRB(Harga Berlaku, Juta Rupiah)</t>
+  </si>
+  <si>
+    <t>PDRB(Harga 2010, Juta Rupiah)</t>
+  </si>
+  <si>
+    <t>Tenaga Kerja 15 th Ke Atas (Orang)</t>
+  </si>
+  <si>
+    <t>Laju PDRB (Harga 2010, % Per Tahun)</t>
   </si>
 </sst>
 </file>
@@ -444,7 +807,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0.000000_);_(* \(#,##0.000000\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.0000000000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -495,6 +858,19 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -628,7 +1004,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -709,6 +1085,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -721,17 +1103,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3006,7 +3409,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F5B0A35-D970-4535-B6B0-E5AD36F4652D}">
   <dimension ref="A1:V22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="A6" sqref="A6"/>
     </sheetView>
@@ -4172,10 +4575,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="43"/>
+      <c r="C1" s="45"/>
       <c r="D1" s="46" t="s">
         <v>41</v>
       </c>
@@ -4898,6 +5301,2056 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C0E5AFA-6774-49D4-9F86-9C5D12637256}">
+  <dimension ref="A1:N27"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M25" sqref="M25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="51"/>
+    <col min="2" max="2" width="24.85546875" style="49" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="51" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" style="51" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" style="51" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" style="51" customWidth="1"/>
+    <col min="7" max="7" width="25" style="51" customWidth="1"/>
+    <col min="8" max="8" width="20.28515625" style="51" customWidth="1"/>
+    <col min="9" max="9" width="19.42578125" style="51" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" style="51" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" style="51" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="15.28515625" style="51" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.28515625" style="51" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="51"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" s="49" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1" s="48"/>
+      <c r="B1" s="48" t="s">
+        <v>118</v>
+      </c>
+      <c r="C1" s="48" t="s">
+        <v>119</v>
+      </c>
+      <c r="D1" s="48" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1" s="48" t="s">
+        <v>146</v>
+      </c>
+      <c r="F1" s="48" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1" s="48" t="s">
+        <v>147</v>
+      </c>
+      <c r="H1" s="48" t="s">
+        <v>148</v>
+      </c>
+      <c r="I1" s="48" t="s">
+        <v>149</v>
+      </c>
+      <c r="J1" s="48" t="s">
+        <v>150</v>
+      </c>
+      <c r="K1" s="48" t="s">
+        <v>151</v>
+      </c>
+      <c r="L1" s="48" t="s">
+        <v>152</v>
+      </c>
+      <c r="M1" s="48" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="50">
+        <v>10</v>
+      </c>
+      <c r="B2" s="48" t="s">
+        <v>121</v>
+      </c>
+      <c r="C2" s="50">
+        <v>1055</v>
+      </c>
+      <c r="D2" s="50">
+        <v>106055</v>
+      </c>
+      <c r="E2" s="50">
+        <v>72246122.290000007</v>
+      </c>
+      <c r="F2" s="50">
+        <v>49475992.210000001</v>
+      </c>
+      <c r="G2" s="50">
+        <v>22770130.079999998</v>
+      </c>
+      <c r="H2" s="53">
+        <v>40739853.259999998</v>
+      </c>
+      <c r="I2" s="53">
+        <v>2832305.8849999998</v>
+      </c>
+      <c r="J2" s="53">
+        <v>2523273.4589999998</v>
+      </c>
+      <c r="K2" s="53">
+        <v>316101.196</v>
+      </c>
+      <c r="L2" s="53">
+        <v>3064458.406</v>
+      </c>
+      <c r="M2" s="53">
+        <v>3380559.602</v>
+      </c>
+      <c r="N2" s="55"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="50">
+        <v>11</v>
+      </c>
+      <c r="B3" s="48" t="s">
+        <v>122</v>
+      </c>
+      <c r="C3" s="50">
+        <v>96</v>
+      </c>
+      <c r="D3" s="50">
+        <v>17158</v>
+      </c>
+      <c r="E3" s="50">
+        <v>8273813.6100000003</v>
+      </c>
+      <c r="F3" s="50">
+        <v>3519664.4249999998</v>
+      </c>
+      <c r="G3" s="50">
+        <v>4754149.1869999999</v>
+      </c>
+      <c r="H3" s="53">
+        <v>2546384.361</v>
+      </c>
+      <c r="I3" s="53">
+        <v>136708.09299999999</v>
+      </c>
+      <c r="J3" s="53">
+        <v>169296.01199999999</v>
+      </c>
+      <c r="K3" s="53">
+        <v>38821.398999999998</v>
+      </c>
+      <c r="L3" s="53">
+        <v>628454.56000000006</v>
+      </c>
+      <c r="M3" s="53">
+        <v>667275.95900000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="50">
+        <v>12</v>
+      </c>
+      <c r="B4" s="48" t="s">
+        <v>123</v>
+      </c>
+      <c r="C4" s="50">
+        <v>9</v>
+      </c>
+      <c r="D4" s="50">
+        <v>1478</v>
+      </c>
+      <c r="E4" s="50">
+        <v>165278.64000000001</v>
+      </c>
+      <c r="F4" s="50">
+        <v>53845.83</v>
+      </c>
+      <c r="G4" s="50">
+        <v>111432.81</v>
+      </c>
+      <c r="H4" s="53">
+        <v>48259.381999999998</v>
+      </c>
+      <c r="I4" s="53">
+        <v>507.137</v>
+      </c>
+      <c r="J4" s="53">
+        <v>315.36</v>
+      </c>
+      <c r="K4" s="53">
+        <v>447.23700000000002</v>
+      </c>
+      <c r="L4" s="53">
+        <v>4316.7139999999999</v>
+      </c>
+      <c r="M4" s="53">
+        <v>4763.951</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="50">
+        <v>13</v>
+      </c>
+      <c r="B5" s="48" t="s">
+        <v>126</v>
+      </c>
+      <c r="C5" s="50">
+        <v>1088</v>
+      </c>
+      <c r="D5" s="50">
+        <v>261913</v>
+      </c>
+      <c r="E5" s="50">
+        <v>191901569.88</v>
+      </c>
+      <c r="F5" s="50">
+        <v>136688262.80000001</v>
+      </c>
+      <c r="G5" s="50">
+        <v>55213307.049999997</v>
+      </c>
+      <c r="H5" s="53">
+        <v>106226924</v>
+      </c>
+      <c r="I5" s="53">
+        <v>4844760.0939999996</v>
+      </c>
+      <c r="J5" s="53">
+        <v>16845928.920000002</v>
+      </c>
+      <c r="K5" s="53">
+        <v>505929.80300000001</v>
+      </c>
+      <c r="L5" s="53">
+        <v>8264720.0060000001</v>
+      </c>
+      <c r="M5" s="53">
+        <v>8770649.8090000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="50">
+        <v>14</v>
+      </c>
+      <c r="B6" s="48" t="s">
+        <v>124</v>
+      </c>
+      <c r="C6" s="50">
+        <v>792</v>
+      </c>
+      <c r="D6" s="50">
+        <v>308237</v>
+      </c>
+      <c r="E6" s="50">
+        <v>67966121.480000004</v>
+      </c>
+      <c r="F6" s="50">
+        <v>36977500.460000001</v>
+      </c>
+      <c r="G6" s="50">
+        <v>30988621.02</v>
+      </c>
+      <c r="H6" s="53">
+        <v>25770954.780000001</v>
+      </c>
+      <c r="I6" s="53">
+        <v>1737878.037</v>
+      </c>
+      <c r="J6" s="53">
+        <v>2875932.1690000002</v>
+      </c>
+      <c r="K6" s="53">
+        <v>1255541.7990000001</v>
+      </c>
+      <c r="L6" s="53">
+        <v>5337193.6840000004</v>
+      </c>
+      <c r="M6" s="53">
+        <v>6592735.483</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="50">
+        <v>15</v>
+      </c>
+      <c r="B7" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="C7" s="50">
+        <v>217</v>
+      </c>
+      <c r="D7" s="50">
+        <v>114133</v>
+      </c>
+      <c r="E7" s="50">
+        <v>28944889.18</v>
+      </c>
+      <c r="F7" s="50">
+        <v>6813613.8729999997</v>
+      </c>
+      <c r="G7" s="50">
+        <v>22131275.300000001</v>
+      </c>
+      <c r="H7" s="53">
+        <v>5278807.9670000002</v>
+      </c>
+      <c r="I7" s="53">
+        <v>268820.59499999997</v>
+      </c>
+      <c r="J7" s="53">
+        <v>650807.397</v>
+      </c>
+      <c r="K7" s="53">
+        <v>55551.146000000001</v>
+      </c>
+      <c r="L7" s="53">
+        <v>559626.76800000004</v>
+      </c>
+      <c r="M7" s="53">
+        <v>615177.91399999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="50">
+        <v>16</v>
+      </c>
+      <c r="B8" s="48" t="s">
+        <v>127</v>
+      </c>
+      <c r="C8" s="50">
+        <v>134</v>
+      </c>
+      <c r="D8" s="50">
+        <v>24838</v>
+      </c>
+      <c r="E8" s="50">
+        <v>4182718</v>
+      </c>
+      <c r="F8" s="50">
+        <v>2409949</v>
+      </c>
+      <c r="G8" s="50">
+        <v>1772770</v>
+      </c>
+      <c r="H8" s="54">
+        <v>2032028.399</v>
+      </c>
+      <c r="I8" s="54">
+        <v>93780.304000000004</v>
+      </c>
+      <c r="J8" s="54">
+        <v>123766.724</v>
+      </c>
+      <c r="K8" s="54">
+        <v>14209.503000000001</v>
+      </c>
+      <c r="L8" s="54">
+        <v>146163.842</v>
+      </c>
+      <c r="M8" s="54">
+        <v>160373.345</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="50">
+        <v>17</v>
+      </c>
+      <c r="B9" s="48" t="s">
+        <v>128</v>
+      </c>
+      <c r="C9" s="50">
+        <v>105</v>
+      </c>
+      <c r="D9" s="50">
+        <v>26805</v>
+      </c>
+      <c r="E9" s="50"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="54">
+        <v>19204551.41</v>
+      </c>
+      <c r="I9" s="54">
+        <v>3867666.8909999998</v>
+      </c>
+      <c r="J9" s="54">
+        <v>2283822.8939999999</v>
+      </c>
+      <c r="K9" s="54">
+        <v>78771.990999999995</v>
+      </c>
+      <c r="L9" s="54">
+        <v>1158831.9339999999</v>
+      </c>
+      <c r="M9" s="54">
+        <v>1237603.925</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="50">
+        <v>18</v>
+      </c>
+      <c r="B10" s="48" t="s">
+        <v>129</v>
+      </c>
+      <c r="C10" s="50">
+        <v>95</v>
+      </c>
+      <c r="D10" s="50">
+        <v>12900</v>
+      </c>
+      <c r="E10" s="50">
+        <v>49787693</v>
+      </c>
+      <c r="F10" s="50">
+        <v>26593645</v>
+      </c>
+      <c r="G10" s="50">
+        <v>23194048</v>
+      </c>
+      <c r="H10" s="54">
+        <v>2588472.952</v>
+      </c>
+      <c r="I10" s="54">
+        <v>196359.07500000001</v>
+      </c>
+      <c r="J10" s="54">
+        <v>828347.61100000003</v>
+      </c>
+      <c r="K10" s="54">
+        <v>57096.451000000001</v>
+      </c>
+      <c r="L10" s="54">
+        <v>314004.59299999999</v>
+      </c>
+      <c r="M10" s="54">
+        <v>371101.04399999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="50">
+        <v>19</v>
+      </c>
+      <c r="B11" s="48" t="s">
+        <v>130</v>
+      </c>
+      <c r="C11" s="50">
+        <v>15</v>
+      </c>
+      <c r="D11" s="50">
+        <v>1121</v>
+      </c>
+      <c r="E11" s="50">
+        <v>9138129</v>
+      </c>
+      <c r="F11" s="50">
+        <v>3984281</v>
+      </c>
+      <c r="G11" s="50">
+        <v>5153848</v>
+      </c>
+      <c r="H11" s="54">
+        <v>228367.027</v>
+      </c>
+      <c r="I11" s="54">
+        <v>16751.103999999999</v>
+      </c>
+      <c r="J11" s="54">
+        <v>5644.5540000000001</v>
+      </c>
+      <c r="K11" s="54">
+        <v>6403.7529999999997</v>
+      </c>
+      <c r="L11" s="54">
+        <v>10740.710999999999</v>
+      </c>
+      <c r="M11" s="54">
+        <v>17144.464</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="50">
+        <v>20</v>
+      </c>
+      <c r="B12" s="48" t="s">
+        <v>131</v>
+      </c>
+      <c r="C12" s="50">
+        <v>305</v>
+      </c>
+      <c r="D12" s="50">
+        <v>56816</v>
+      </c>
+      <c r="E12" s="50">
+        <v>163974828</v>
+      </c>
+      <c r="F12" s="50">
+        <v>110171293</v>
+      </c>
+      <c r="G12" s="50">
+        <v>53803535</v>
+      </c>
+      <c r="H12" s="54">
+        <v>77876445.849999994</v>
+      </c>
+      <c r="I12" s="54">
+        <v>3366995.986</v>
+      </c>
+      <c r="J12" s="54">
+        <v>12704461.59</v>
+      </c>
+      <c r="K12" s="54">
+        <v>1098247.0120000001</v>
+      </c>
+      <c r="L12" s="54">
+        <v>15125142.279999999</v>
+      </c>
+      <c r="M12" s="54">
+        <v>16223389.300000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="50">
+        <v>21</v>
+      </c>
+      <c r="B13" s="48" t="s">
+        <v>133</v>
+      </c>
+      <c r="C13" s="50">
+        <v>76</v>
+      </c>
+      <c r="D13" s="50">
+        <v>17793</v>
+      </c>
+      <c r="E13" s="50">
+        <v>13347012</v>
+      </c>
+      <c r="F13" s="50">
+        <v>6653139</v>
+      </c>
+      <c r="G13" s="50">
+        <v>6693873</v>
+      </c>
+      <c r="H13" s="54">
+        <v>3557162.963</v>
+      </c>
+      <c r="I13" s="54">
+        <v>796940.30599999998</v>
+      </c>
+      <c r="J13" s="54">
+        <v>301258.38099999999</v>
+      </c>
+      <c r="K13" s="54">
+        <v>46683.519999999997</v>
+      </c>
+      <c r="L13" s="54">
+        <v>1951094.24</v>
+      </c>
+      <c r="M13" s="54">
+        <v>1997777.76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="50">
+        <v>22</v>
+      </c>
+      <c r="B14" s="48" t="s">
+        <v>132</v>
+      </c>
+      <c r="C14" s="50">
+        <v>482</v>
+      </c>
+      <c r="D14" s="50">
+        <v>168930</v>
+      </c>
+      <c r="E14" s="50">
+        <v>0</v>
+      </c>
+      <c r="F14" s="50">
+        <v>0</v>
+      </c>
+      <c r="G14" s="50">
+        <v>0</v>
+      </c>
+      <c r="H14" s="54">
+        <v>55610127.700000003</v>
+      </c>
+      <c r="I14" s="54">
+        <v>4586907.1500000004</v>
+      </c>
+      <c r="J14" s="54">
+        <v>4135991.5019999999</v>
+      </c>
+      <c r="K14" s="54">
+        <v>467095.97200000001</v>
+      </c>
+      <c r="L14" s="54">
+        <v>5317320.8930000002</v>
+      </c>
+      <c r="M14" s="54">
+        <v>5784416.8650000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="50">
+        <v>23</v>
+      </c>
+      <c r="B15" s="48" t="s">
+        <v>134</v>
+      </c>
+      <c r="C15" s="50">
+        <v>746</v>
+      </c>
+      <c r="D15" s="50">
+        <v>73212</v>
+      </c>
+      <c r="E15" s="50">
+        <v>119705692</v>
+      </c>
+      <c r="F15" s="50">
+        <v>70117443</v>
+      </c>
+      <c r="G15" s="50">
+        <v>49588249</v>
+      </c>
+      <c r="H15" s="54">
+        <v>8500021.9609999992</v>
+      </c>
+      <c r="I15" s="54">
+        <v>2556858.4079999998</v>
+      </c>
+      <c r="J15" s="54">
+        <v>1177682.956</v>
+      </c>
+      <c r="K15" s="54">
+        <v>50720.622000000003</v>
+      </c>
+      <c r="L15" s="54">
+        <v>818403.66599999997</v>
+      </c>
+      <c r="M15" s="54">
+        <v>869124.28799999994</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="50">
+        <v>24</v>
+      </c>
+      <c r="B16" s="48" t="s">
+        <v>135</v>
+      </c>
+      <c r="C16" s="50">
+        <v>86</v>
+      </c>
+      <c r="D16" s="50">
+        <v>13366</v>
+      </c>
+      <c r="E16" s="50">
+        <v>28795098</v>
+      </c>
+      <c r="F16" s="50">
+        <v>16564823</v>
+      </c>
+      <c r="G16" s="50">
+        <v>12230275</v>
+      </c>
+      <c r="H16" s="54">
+        <v>22190069.120000001</v>
+      </c>
+      <c r="I16" s="54">
+        <v>440065.90600000002</v>
+      </c>
+      <c r="J16" s="54">
+        <v>766064.65399999998</v>
+      </c>
+      <c r="K16" s="54">
+        <v>80086.557000000001</v>
+      </c>
+      <c r="L16" s="54">
+        <v>754530.20200000005</v>
+      </c>
+      <c r="M16" s="54">
+        <v>834616.75899999996</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="50">
+        <v>25</v>
+      </c>
+      <c r="B17" s="48" t="s">
+        <v>136</v>
+      </c>
+      <c r="C17" s="50">
+        <v>293</v>
+      </c>
+      <c r="D17" s="50">
+        <v>45322</v>
+      </c>
+      <c r="E17" s="50">
+        <v>110719139</v>
+      </c>
+      <c r="F17" s="50">
+        <v>65588105</v>
+      </c>
+      <c r="G17" s="50">
+        <v>45131034</v>
+      </c>
+      <c r="H17" s="54">
+        <v>12450684.369999999</v>
+      </c>
+      <c r="I17" s="54">
+        <v>669150.76699999999</v>
+      </c>
+      <c r="J17" s="54">
+        <v>968209.82799999998</v>
+      </c>
+      <c r="K17" s="54">
+        <v>966258.54099999997</v>
+      </c>
+      <c r="L17" s="54">
+        <v>1510519.166</v>
+      </c>
+      <c r="M17" s="54">
+        <v>16564822.67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="50">
+        <v>26</v>
+      </c>
+      <c r="B18" s="48" t="s">
+        <v>137</v>
+      </c>
+      <c r="C18" s="50">
+        <v>191</v>
+      </c>
+      <c r="D18" s="50">
+        <v>77590</v>
+      </c>
+      <c r="E18" s="50">
+        <v>0</v>
+      </c>
+      <c r="F18" s="50">
+        <v>0</v>
+      </c>
+      <c r="G18" s="50">
+        <v>0</v>
+      </c>
+      <c r="H18" s="54">
+        <v>56732802.280000001</v>
+      </c>
+      <c r="I18" s="54">
+        <v>739942.25899999996</v>
+      </c>
+      <c r="J18" s="54">
+        <v>3722548.1310000001</v>
+      </c>
+      <c r="K18" s="54">
+        <v>669401.68200000003</v>
+      </c>
+      <c r="L18" s="54">
+        <v>3723410.5839999998</v>
+      </c>
+      <c r="M18" s="54">
+        <v>65588104.939999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="50">
+        <v>27</v>
+      </c>
+      <c r="B19" s="48" t="s">
+        <v>138</v>
+      </c>
+      <c r="C19" s="50">
+        <v>139</v>
+      </c>
+      <c r="D19" s="50">
+        <v>43485</v>
+      </c>
+      <c r="E19" s="50">
+        <v>60125184</v>
+      </c>
+      <c r="F19" s="50">
+        <v>28148439</v>
+      </c>
+      <c r="G19" s="50">
+        <v>31976745</v>
+      </c>
+      <c r="H19" s="54">
+        <v>22752740</v>
+      </c>
+      <c r="I19" s="54">
+        <v>936541.446</v>
+      </c>
+      <c r="J19" s="54">
+        <v>2406596.3790000002</v>
+      </c>
+      <c r="K19" s="54">
+        <v>799239.57499999995</v>
+      </c>
+      <c r="L19" s="54">
+        <v>1253321.1129999999</v>
+      </c>
+      <c r="M19" s="54">
+        <v>28148438.510000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="50">
+        <v>28</v>
+      </c>
+      <c r="B20" s="48" t="s">
+        <v>139</v>
+      </c>
+      <c r="C20" s="50">
+        <v>172</v>
+      </c>
+      <c r="D20" s="50">
+        <v>32630</v>
+      </c>
+      <c r="E20" s="50">
+        <v>38530958</v>
+      </c>
+      <c r="F20" s="50">
+        <v>15183535</v>
+      </c>
+      <c r="G20" s="50">
+        <v>23347423</v>
+      </c>
+      <c r="H20" s="54">
+        <v>10367254.18</v>
+      </c>
+      <c r="I20" s="54">
+        <v>227815.905</v>
+      </c>
+      <c r="J20" s="54">
+        <v>530874.05000000005</v>
+      </c>
+      <c r="K20" s="54">
+        <v>66269.418999999994</v>
+      </c>
+      <c r="L20" s="54">
+        <v>3991321.196</v>
+      </c>
+      <c r="M20" s="54">
+        <v>15183534.75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="50">
+        <v>29</v>
+      </c>
+      <c r="B21" s="48" t="s">
+        <v>144</v>
+      </c>
+      <c r="C21" s="50">
+        <v>10</v>
+      </c>
+      <c r="D21" s="50">
+        <v>0</v>
+      </c>
+      <c r="E21" s="50">
+        <v>199790543</v>
+      </c>
+      <c r="F21" s="50">
+        <v>92991681</v>
+      </c>
+      <c r="G21" s="50">
+        <v>106798862</v>
+      </c>
+      <c r="H21" s="54">
+        <v>65350406.479999997</v>
+      </c>
+      <c r="I21" s="54">
+        <v>2327436.7969999998</v>
+      </c>
+      <c r="J21" s="54">
+        <v>5039601.415</v>
+      </c>
+      <c r="K21" s="54">
+        <v>565426.52899999998</v>
+      </c>
+      <c r="L21" s="54">
+        <v>19708809.350000001</v>
+      </c>
+      <c r="M21" s="54">
+        <v>92991680.569999993</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="50">
+        <v>30</v>
+      </c>
+      <c r="B22" s="48" t="s">
+        <v>140</v>
+      </c>
+      <c r="C22" s="50">
+        <v>233</v>
+      </c>
+      <c r="D22" s="50">
+        <v>74059</v>
+      </c>
+      <c r="E22" s="50">
+        <v>21099427</v>
+      </c>
+      <c r="F22" s="50">
+        <v>10464566</v>
+      </c>
+      <c r="G22" s="50">
+        <v>10634861</v>
+      </c>
+      <c r="H22" s="54">
+        <v>7829314.6909999996</v>
+      </c>
+      <c r="I22" s="54">
+        <v>411032.09100000001</v>
+      </c>
+      <c r="J22" s="54">
+        <v>807386.43099999998</v>
+      </c>
+      <c r="K22" s="54">
+        <v>628950.14</v>
+      </c>
+      <c r="L22" s="54">
+        <v>787882.87100000004</v>
+      </c>
+      <c r="M22" s="54">
+        <v>10464566.220000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="50">
+        <v>31</v>
+      </c>
+      <c r="B23" s="48" t="s">
+        <v>141</v>
+      </c>
+      <c r="C23" s="50">
+        <v>129</v>
+      </c>
+      <c r="D23" s="50">
+        <v>29350</v>
+      </c>
+      <c r="E23" s="50">
+        <v>10011628</v>
+      </c>
+      <c r="F23" s="50">
+        <v>5280536</v>
+      </c>
+      <c r="G23" s="50">
+        <v>4731092</v>
+      </c>
+      <c r="H23" s="54">
+        <v>3738679.6290000002</v>
+      </c>
+      <c r="I23" s="54">
+        <v>196400.247</v>
+      </c>
+      <c r="J23" s="54">
+        <v>407711.35499999998</v>
+      </c>
+      <c r="K23" s="54">
+        <v>342018.21799999999</v>
+      </c>
+      <c r="L23" s="54">
+        <v>595726.53700000001</v>
+      </c>
+      <c r="M23" s="54">
+        <v>5280535.9859999996</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="50">
+        <v>32</v>
+      </c>
+      <c r="B24" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="C24" s="50">
+        <v>251</v>
+      </c>
+      <c r="D24" s="50">
+        <v>31858</v>
+      </c>
+      <c r="E24" s="50">
+        <v>0</v>
+      </c>
+      <c r="F24" s="50">
+        <v>0</v>
+      </c>
+      <c r="G24" s="50">
+        <v>0</v>
+      </c>
+      <c r="H24" s="54">
+        <v>4259563.3760000002</v>
+      </c>
+      <c r="I24" s="54">
+        <v>175390.073</v>
+      </c>
+      <c r="J24" s="54">
+        <v>250364.48</v>
+      </c>
+      <c r="K24" s="54">
+        <v>186701.245</v>
+      </c>
+      <c r="L24" s="54">
+        <v>339721.91200000001</v>
+      </c>
+      <c r="M24" s="54">
+        <v>5211741.0860000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="50">
+        <v>33</v>
+      </c>
+      <c r="B25" s="48" t="s">
+        <v>143</v>
+      </c>
+      <c r="C25" s="50">
+        <v>155</v>
+      </c>
+      <c r="D25" s="50">
+        <v>51383</v>
+      </c>
+      <c r="E25" s="50">
+        <v>16398625</v>
+      </c>
+      <c r="F25" s="50">
+        <v>5211741</v>
+      </c>
+      <c r="G25" s="50">
+        <v>11186884</v>
+      </c>
+      <c r="H25" s="54">
+        <v>21035.981</v>
+      </c>
+      <c r="I25" s="54">
+        <v>12383.26</v>
+      </c>
+      <c r="J25" s="54">
+        <v>5396.2420000000002</v>
+      </c>
+      <c r="K25" s="54">
+        <v>1845.67</v>
+      </c>
+      <c r="L25" s="54">
+        <v>11347.286</v>
+      </c>
+      <c r="M25" s="54">
+        <v>52008.438999999998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="52" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" s="52"/>
+      <c r="C26" s="50">
+        <v>6874</v>
+      </c>
+      <c r="D26" s="50">
+        <v>1588155</v>
+      </c>
+      <c r="E26" s="50">
+        <v>1215104469.0799999</v>
+      </c>
+      <c r="F26" s="50">
+        <v>692892005.74000001</v>
+      </c>
+      <c r="G26" s="50">
+        <v>522212414.44999999</v>
+      </c>
+      <c r="H26" s="53">
+        <v>555900912</v>
+      </c>
+      <c r="I26" s="53">
+        <v>31439398</v>
+      </c>
+      <c r="J26" s="53">
+        <v>59531283</v>
+      </c>
+      <c r="K26" s="53">
+        <v>8297819</v>
+      </c>
+      <c r="L26" s="53">
+        <v>75377063</v>
+      </c>
+      <c r="M26" s="53">
+        <v>730546474</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="50"/>
+      <c r="B27" s="48"/>
+      <c r="C27" s="50">
+        <f>SUM(C2:C25)</f>
+        <v>6874</v>
+      </c>
+      <c r="D27" s="50">
+        <f>SUM(D2:D25)</f>
+        <v>1590432</v>
+      </c>
+      <c r="E27" s="50">
+        <f t="shared" ref="E27:M27" si="0">SUM(E2:E25)</f>
+        <v>1215104469.0799999</v>
+      </c>
+      <c r="F27" s="50">
+        <f t="shared" si="0"/>
+        <v>692892055.59800005</v>
+      </c>
+      <c r="G27" s="50">
+        <f t="shared" si="0"/>
+        <v>522212414.44700003</v>
+      </c>
+      <c r="H27" s="53">
+        <f t="shared" si="0"/>
+        <v>555900912.11899996</v>
+      </c>
+      <c r="I27" s="53">
+        <f t="shared" si="0"/>
+        <v>31439397.815999996</v>
+      </c>
+      <c r="J27" s="53">
+        <f t="shared" si="0"/>
+        <v>59531282.493999988</v>
+      </c>
+      <c r="K27" s="53">
+        <f t="shared" si="0"/>
+        <v>8297818.9800000004</v>
+      </c>
+      <c r="L27" s="53">
+        <f t="shared" si="0"/>
+        <v>75377062.513999999</v>
+      </c>
+      <c r="M27" s="53">
+        <f>SUM(M2:M25)</f>
+        <v>287012143.63900006</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A26:B26"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D20A539-ECC7-4EF4-8565-B3E0F3F6B1AB}">
+  <dimension ref="A1:AA32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="T1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AA13" sqref="AA13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" customWidth="1"/>
+    <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9" customWidth="1"/>
+    <col min="13" max="13" width="6.85546875" customWidth="1"/>
+    <col min="24" max="24" width="18.42578125" customWidth="1"/>
+    <col min="25" max="25" width="21.28515625" customWidth="1"/>
+    <col min="26" max="26" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="17.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" s="49" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H1" s="56" t="s">
+        <v>159</v>
+      </c>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56" t="s">
+        <v>167</v>
+      </c>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56" t="s">
+        <v>168</v>
+      </c>
+      <c r="M1" s="56"/>
+      <c r="N1" s="56" t="s">
+        <v>162</v>
+      </c>
+      <c r="O1" s="56"/>
+      <c r="P1" s="56" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q1" s="56"/>
+      <c r="R1" s="56" t="s">
+        <v>164</v>
+      </c>
+      <c r="S1" s="56"/>
+      <c r="T1" s="36" t="s">
+        <v>165</v>
+      </c>
+      <c r="U1" s="36"/>
+      <c r="V1" s="36" t="s">
+        <v>166</v>
+      </c>
+      <c r="W1" s="36"/>
+      <c r="X1" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" s="49" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="49" t="s">
+        <v>153</v>
+      </c>
+      <c r="C2" s="49" t="s">
+        <v>154</v>
+      </c>
+      <c r="D2" s="49" t="s">
+        <v>155</v>
+      </c>
+      <c r="E2" s="49" t="s">
+        <v>156</v>
+      </c>
+      <c r="F2" s="49" t="s">
+        <v>157</v>
+      </c>
+      <c r="G2" s="49" t="s">
+        <v>158</v>
+      </c>
+      <c r="H2" s="49" t="s">
+        <v>160</v>
+      </c>
+      <c r="I2" s="49" t="s">
+        <v>161</v>
+      </c>
+      <c r="J2" s="49" t="s">
+        <v>160</v>
+      </c>
+      <c r="K2" s="49" t="s">
+        <v>161</v>
+      </c>
+      <c r="L2" s="49" t="s">
+        <v>160</v>
+      </c>
+      <c r="M2" s="49" t="s">
+        <v>161</v>
+      </c>
+      <c r="N2" s="49" t="s">
+        <v>160</v>
+      </c>
+      <c r="O2" s="49" t="s">
+        <v>161</v>
+      </c>
+      <c r="P2" s="49" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q2" s="49" t="s">
+        <v>161</v>
+      </c>
+      <c r="R2" s="49" t="s">
+        <v>160</v>
+      </c>
+      <c r="S2" s="49" t="s">
+        <v>161</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
+    </row>
+    <row r="3" spans="1:27" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2008</v>
+      </c>
+      <c r="H3" s="49">
+        <v>156482</v>
+      </c>
+      <c r="I3" s="49">
+        <v>13594</v>
+      </c>
+      <c r="J3" s="49">
+        <v>68344</v>
+      </c>
+      <c r="L3" s="49">
+        <v>496857</v>
+      </c>
+      <c r="M3" s="49">
+        <v>88847</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N6" si="0">H3+J3+L3</f>
+        <v>721683</v>
+      </c>
+      <c r="O3">
+        <f t="shared" ref="O3:O6" si="1">I3+K3+M3</f>
+        <v>102441</v>
+      </c>
+      <c r="P3" s="49">
+        <v>10452</v>
+      </c>
+      <c r="Q3" s="49">
+        <v>16448</v>
+      </c>
+      <c r="R3" s="49">
+        <v>284287</v>
+      </c>
+      <c r="S3" s="49">
+        <v>13179</v>
+      </c>
+      <c r="T3" s="2">
+        <v>118</v>
+      </c>
+      <c r="U3" s="2">
+        <v>34</v>
+      </c>
+      <c r="V3" s="2">
+        <v>5818657</v>
+      </c>
+      <c r="W3" s="2">
+        <v>0</v>
+      </c>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2"/>
+      <c r="AA3" s="2"/>
+    </row>
+    <row r="4" spans="1:27" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>2009</v>
+      </c>
+      <c r="H4" s="49">
+        <v>162423</v>
+      </c>
+      <c r="I4" s="49">
+        <v>14311</v>
+      </c>
+      <c r="J4" s="49">
+        <v>70852</v>
+      </c>
+      <c r="L4" s="49">
+        <v>540380</v>
+      </c>
+      <c r="M4" s="49">
+        <v>89602</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="0"/>
+        <v>773655</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="1"/>
+        <v>103913</v>
+      </c>
+      <c r="P4" s="49">
+        <v>10622</v>
+      </c>
+      <c r="Q4" s="49">
+        <v>17493</v>
+      </c>
+      <c r="R4" s="49">
+        <v>293429</v>
+      </c>
+      <c r="S4" s="49">
+        <v>19401</v>
+      </c>
+      <c r="T4" s="2">
+        <v>125</v>
+      </c>
+      <c r="U4" s="2">
+        <v>36</v>
+      </c>
+      <c r="V4" s="2">
+        <v>6775893</v>
+      </c>
+      <c r="W4" s="14">
+        <v>0</v>
+      </c>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2"/>
+      <c r="Z4" s="2"/>
+      <c r="AA4" s="2"/>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A5" s="14">
+        <v>2010</v>
+      </c>
+      <c r="B5">
+        <v>43227107</v>
+      </c>
+      <c r="H5">
+        <v>168292</v>
+      </c>
+      <c r="I5">
+        <v>13842</v>
+      </c>
+      <c r="J5">
+        <v>74968</v>
+      </c>
+      <c r="K5">
+        <v>4</v>
+      </c>
+      <c r="L5">
+        <v>627276</v>
+      </c>
+      <c r="M5">
+        <v>71513</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="0"/>
+        <v>870536</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="1"/>
+        <v>85359</v>
+      </c>
+      <c r="P5">
+        <v>7209</v>
+      </c>
+      <c r="Q5" s="31">
+        <v>16375</v>
+      </c>
+      <c r="R5">
+        <v>300790</v>
+      </c>
+      <c r="S5">
+        <v>19401</v>
+      </c>
+      <c r="T5" s="14">
+        <v>68</v>
+      </c>
+      <c r="U5" s="14">
+        <v>10</v>
+      </c>
+      <c r="V5" s="14">
+        <v>7636482</v>
+      </c>
+      <c r="W5" s="14">
+        <v>0</v>
+      </c>
+      <c r="X5" s="14">
+        <v>3389287</v>
+      </c>
+      <c r="Y5" s="14">
+        <v>291688080</v>
+      </c>
+      <c r="Z5" s="14"/>
+      <c r="AA5" s="14"/>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A6" s="14">
+        <v>2011</v>
+      </c>
+      <c r="B6">
+        <v>43938796</v>
+      </c>
+      <c r="H6">
+        <v>163185</v>
+      </c>
+      <c r="I6">
+        <v>14870</v>
+      </c>
+      <c r="J6">
+        <v>78212</v>
+      </c>
+      <c r="K6">
+        <v>3</v>
+      </c>
+      <c r="L6">
+        <v>689990</v>
+      </c>
+      <c r="M6">
+        <v>68896</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="0"/>
+        <v>931387</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="1"/>
+        <v>83769</v>
+      </c>
+      <c r="P6">
+        <v>7467</v>
+      </c>
+      <c r="Q6">
+        <v>16995</v>
+      </c>
+      <c r="R6">
+        <v>312050</v>
+      </c>
+      <c r="S6">
+        <v>22161</v>
+      </c>
+      <c r="T6" s="14">
+        <v>79</v>
+      </c>
+      <c r="U6" s="14">
+        <v>15</v>
+      </c>
+      <c r="V6" s="14">
+        <v>8426228</v>
+      </c>
+      <c r="W6" s="14">
+        <v>0</v>
+      </c>
+      <c r="X6" s="14"/>
+      <c r="Y6" s="14">
+        <v>319983632</v>
+      </c>
+      <c r="Z6" s="14"/>
+      <c r="AA6" s="14"/>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A7" s="14">
+        <v>2012</v>
+      </c>
+      <c r="B7">
+        <v>44643586</v>
+      </c>
+      <c r="H7">
+        <v>1070433</v>
+      </c>
+      <c r="I7">
+        <v>86373</v>
+      </c>
+      <c r="N7">
+        <f>H7+J7+L7</f>
+        <v>1070433</v>
+      </c>
+      <c r="O7">
+        <f>I7+K7+M7</f>
+        <v>86373</v>
+      </c>
+      <c r="P7">
+        <v>7123</v>
+      </c>
+      <c r="Q7">
+        <v>17837</v>
+      </c>
+      <c r="R7">
+        <v>346859</v>
+      </c>
+      <c r="S7">
+        <v>29896</v>
+      </c>
+      <c r="T7" s="14">
+        <v>66</v>
+      </c>
+      <c r="U7" s="14">
+        <v>17</v>
+      </c>
+      <c r="V7" s="14">
+        <v>9626748</v>
+      </c>
+      <c r="W7" s="14">
+        <v>0</v>
+      </c>
+      <c r="X7" s="14"/>
+      <c r="Y7" s="14">
+        <v>338881030</v>
+      </c>
+      <c r="Z7" s="14"/>
+      <c r="AA7" s="14"/>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A8" s="14">
+        <v>2013</v>
+      </c>
+      <c r="B8">
+        <v>45340799</v>
+      </c>
+      <c r="H8">
+        <v>175654</v>
+      </c>
+      <c r="I8">
+        <v>15916</v>
+      </c>
+      <c r="J8">
+        <v>99350</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8" s="1">
+        <v>948634</v>
+      </c>
+      <c r="M8">
+        <v>70334</v>
+      </c>
+      <c r="N8">
+        <f>H8+J8+L8</f>
+        <v>1223638</v>
+      </c>
+      <c r="O8">
+        <f>I8+K8+M8</f>
+        <v>86250</v>
+      </c>
+      <c r="P8">
+        <v>7369</v>
+      </c>
+      <c r="Q8">
+        <v>18059</v>
+      </c>
+      <c r="R8">
+        <v>381965</v>
+      </c>
+      <c r="S8">
+        <v>38530</v>
+      </c>
+      <c r="T8" s="14">
+        <v>31</v>
+      </c>
+      <c r="U8" s="14">
+        <v>2</v>
+      </c>
+      <c r="V8" s="14">
+        <v>10668631</v>
+      </c>
+      <c r="W8" s="14">
+        <v>0</v>
+      </c>
+      <c r="X8" s="14"/>
+      <c r="Y8" s="14">
+        <v>369830981</v>
+      </c>
+      <c r="Z8" s="14"/>
+      <c r="AA8" s="14"/>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A9" s="14">
+        <v>2014</v>
+      </c>
+      <c r="B9">
+        <v>45680180</v>
+      </c>
+      <c r="H9">
+        <v>179465</v>
+      </c>
+      <c r="I9">
+        <v>17248</v>
+      </c>
+      <c r="J9">
+        <v>108886</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>1103908</v>
+      </c>
+      <c r="M9">
+        <v>70601</v>
+      </c>
+      <c r="N9">
+        <f>H9+J9+L9</f>
+        <v>1392259</v>
+      </c>
+      <c r="O9">
+        <f>I9+K9+M9</f>
+        <v>87849</v>
+      </c>
+      <c r="P9">
+        <v>8088</v>
+      </c>
+      <c r="Q9">
+        <v>18572</v>
+      </c>
+      <c r="R9">
+        <v>417531</v>
+      </c>
+      <c r="S9">
+        <v>45635</v>
+      </c>
+      <c r="T9" s="14">
+        <v>43</v>
+      </c>
+      <c r="U9" s="14">
+        <v>8</v>
+      </c>
+      <c r="V9" s="14">
+        <v>11750515</v>
+      </c>
+      <c r="W9" s="14">
+        <v>0</v>
+      </c>
+      <c r="X9" s="14"/>
+      <c r="Y9" s="14">
+        <v>604374036</v>
+      </c>
+      <c r="Z9" s="14"/>
+      <c r="AA9" s="14"/>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A10" s="14">
+        <v>2015</v>
+      </c>
+      <c r="B10">
+        <v>46709569</v>
+      </c>
+      <c r="T10" s="14"/>
+      <c r="U10" s="14"/>
+      <c r="V10" s="14"/>
+      <c r="W10" s="14"/>
+      <c r="X10" s="14"/>
+      <c r="Y10" s="14">
+        <v>604374036</v>
+      </c>
+      <c r="Z10" s="14">
+        <f>524466.68*1000</f>
+        <v>524466680.00000006</v>
+      </c>
+      <c r="AA10" s="14"/>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A11" s="14">
+        <v>2016</v>
+      </c>
+      <c r="B11">
+        <v>47379389</v>
+      </c>
+      <c r="N11">
+        <v>1708905</v>
+      </c>
+      <c r="O11">
+        <v>85844</v>
+      </c>
+      <c r="P11">
+        <v>9326</v>
+      </c>
+      <c r="Q11">
+        <v>19890</v>
+      </c>
+      <c r="R11">
+        <v>480166</v>
+      </c>
+      <c r="S11">
+        <v>55342</v>
+      </c>
+      <c r="T11" s="14">
+        <v>47</v>
+      </c>
+      <c r="U11" s="14">
+        <v>10</v>
+      </c>
+      <c r="V11" s="14">
+        <v>13725590</v>
+      </c>
+      <c r="W11" s="14">
+        <v>1</v>
+      </c>
+      <c r="X11" s="14"/>
+      <c r="Y11" s="14">
+        <f>703516.39*1000</f>
+        <v>703516390</v>
+      </c>
+      <c r="Z11" s="14">
+        <f>549471.38*1000</f>
+        <v>549471380</v>
+      </c>
+      <c r="AA11" s="14">
+        <v>4.7699999999999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A12" s="14">
+        <v>2017</v>
+      </c>
+      <c r="B12">
+        <v>48037827</v>
+      </c>
+      <c r="C12" s="4">
+        <v>23467004</v>
+      </c>
+      <c r="D12" s="4">
+        <v>50655175450</v>
+      </c>
+      <c r="E12" s="4">
+        <v>47425445657</v>
+      </c>
+      <c r="F12" s="4">
+        <v>126858647</v>
+      </c>
+      <c r="G12" s="4">
+        <v>2698427195</v>
+      </c>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12">
+        <v>1861360</v>
+      </c>
+      <c r="O12">
+        <v>83745</v>
+      </c>
+      <c r="P12">
+        <v>9977</v>
+      </c>
+      <c r="Q12">
+        <v>20764</v>
+      </c>
+      <c r="R12">
+        <v>503795</v>
+      </c>
+      <c r="S12">
+        <v>59361</v>
+      </c>
+      <c r="T12" s="14">
+        <v>53</v>
+      </c>
+      <c r="U12" s="14">
+        <v>10</v>
+      </c>
+      <c r="V12" s="14">
+        <v>14807363</v>
+      </c>
+      <c r="W12" s="14">
+        <v>137</v>
+      </c>
+      <c r="X12" s="14"/>
+      <c r="Y12" s="14">
+        <f>1000*755387.26</f>
+        <v>755387260</v>
+      </c>
+      <c r="Z12" s="14">
+        <f>578858.48*1000</f>
+        <v>578858480</v>
+      </c>
+      <c r="AA12" s="14">
+        <v>5.35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A13" s="14">
+        <v>2018</v>
+      </c>
+      <c r="B13">
+        <v>48683861</v>
+      </c>
+      <c r="N13">
+        <v>1969168</v>
+      </c>
+      <c r="O13">
+        <v>78434</v>
+      </c>
+      <c r="P13">
+        <v>9851</v>
+      </c>
+      <c r="Q13">
+        <v>20027</v>
+      </c>
+      <c r="R13">
+        <v>499594</v>
+      </c>
+      <c r="S13">
+        <v>62714</v>
+      </c>
+      <c r="T13" s="14">
+        <v>46</v>
+      </c>
+      <c r="U13" s="14">
+        <v>9</v>
+      </c>
+      <c r="V13" s="14">
+        <v>14126095</v>
+      </c>
+      <c r="W13" s="14">
+        <v>205</v>
+      </c>
+      <c r="X13" s="14"/>
+      <c r="Y13" s="14">
+        <f>827301.68*1000</f>
+        <v>827301680</v>
+      </c>
+      <c r="Z13" s="14">
+        <f>1000*616441.68</f>
+        <v>616441680</v>
+      </c>
+      <c r="AA13" s="14">
+        <v>6.49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A14" s="14">
+        <v>2019</v>
+      </c>
+      <c r="B14">
+        <v>49316712</v>
+      </c>
+      <c r="T14" s="14"/>
+      <c r="U14" s="14"/>
+      <c r="V14" s="14"/>
+      <c r="W14" s="14"/>
+      <c r="X14" s="14"/>
+      <c r="Y14" s="14"/>
+      <c r="Z14" s="14"/>
+      <c r="AA14" s="14"/>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A15" s="14">
+        <v>2020</v>
+      </c>
+      <c r="B15">
+        <v>49935858</v>
+      </c>
+      <c r="T15" s="14"/>
+      <c r="U15" s="14"/>
+      <c r="V15" s="14"/>
+      <c r="W15" s="14"/>
+      <c r="X15" s="14"/>
+      <c r="Y15" s="14"/>
+      <c r="Z15" s="14"/>
+      <c r="AA15" s="14"/>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D17" s="13"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>170</v>
+      </c>
+      <c r="C18" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" t="s">
+        <v>172</v>
+      </c>
+      <c r="D19" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="49">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="49">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>2020</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:W1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5579,49 +8032,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="40" t="s">
         <v>100</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
-      <c r="J1" s="44" t="s">
+      <c r="J1" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44" t="s">
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="N1" s="44"/>
+      <c r="N1" s="41"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
-      <c r="Q1" s="42" t="s">
+      <c r="Q1" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="R1" s="42"/>
-      <c r="S1" s="42"/>
-      <c r="T1" s="42"/>
-      <c r="U1" s="42"/>
-      <c r="V1" s="42"/>
-      <c r="W1" s="42"/>
-      <c r="X1" s="42"/>
-      <c r="Y1" s="43" t="s">
+      <c r="R1" s="44"/>
+      <c r="S1" s="44"/>
+      <c r="T1" s="44"/>
+      <c r="U1" s="44"/>
+      <c r="V1" s="44"/>
+      <c r="W1" s="44"/>
+      <c r="X1" s="44"/>
+      <c r="Y1" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="Z1" s="43"/>
-      <c r="AA1" s="43"/>
+      <c r="Z1" s="45"/>
+      <c r="AA1" s="45"/>
     </row>
     <row r="2" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="45"/>
-      <c r="B2" s="45"/>
-      <c r="G2" s="40" t="s">
+      <c r="A2" s="40"/>
+      <c r="B2" s="40"/>
+      <c r="G2" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="40"/>
+      <c r="H2" s="42"/>
       <c r="I2" s="11">
         <v>2000</v>
       </c>
@@ -5736,7 +8189,7 @@
         <f t="shared" ref="B4:B12" si="2">B3*(1+$B$24)</f>
         <v>43520231.496352419</v>
       </c>
-      <c r="C4" s="45" t="s">
+      <c r="C4" s="40" t="s">
         <v>92</v>
       </c>
       <c r="G4" s="1">
@@ -5789,7 +8242,7 @@
         <f t="shared" si="2"/>
         <v>43487564.531457625</v>
       </c>
-      <c r="C5" s="45"/>
+      <c r="C5" s="40"/>
       <c r="G5" s="1">
         <v>3</v>
       </c>
@@ -5840,7 +8293,7 @@
         <f t="shared" si="2"/>
         <v>43454922.086896457</v>
       </c>
-      <c r="C6" s="45"/>
+      <c r="C6" s="40"/>
       <c r="G6" s="1">
         <v>4</v>
       </c>
@@ -5891,7 +8344,7 @@
         <f t="shared" si="2"/>
         <v>43422304.144263558</v>
       </c>
-      <c r="C7" s="45"/>
+      <c r="C7" s="40"/>
       <c r="G7" s="1">
         <v>5</v>
       </c>
@@ -5942,7 +8395,7 @@
         <f t="shared" si="2"/>
         <v>43389710.685167402</v>
       </c>
-      <c r="C8" s="45"/>
+      <c r="C8" s="40"/>
       <c r="G8" s="1">
         <v>6</v>
       </c>
@@ -5993,7 +8446,7 @@
         <f t="shared" si="2"/>
         <v>43357141.691230267</v>
       </c>
-      <c r="C9" s="45"/>
+      <c r="C9" s="40"/>
       <c r="G9" s="1">
         <v>7</v>
       </c>
@@ -6044,7 +8497,7 @@
         <f t="shared" si="2"/>
         <v>43324597.144088216</v>
       </c>
-      <c r="C10" s="45"/>
+      <c r="C10" s="40"/>
       <c r="G10" s="1">
         <v>8</v>
       </c>
@@ -6095,7 +8548,7 @@
         <f t="shared" si="2"/>
         <v>43292077.025391109</v>
       </c>
-      <c r="C11" s="45"/>
+      <c r="C11" s="40"/>
       <c r="G11" s="1">
         <v>9</v>
       </c>
@@ -6146,7 +8599,7 @@
         <f t="shared" si="2"/>
         <v>43259581.316802576</v>
       </c>
-      <c r="C12" s="45"/>
+      <c r="C12" s="40"/>
       <c r="G12" s="1">
         <v>10</v>
       </c>
@@ -6197,7 +8650,7 @@
         <f>Q31</f>
         <v>43227110</v>
       </c>
-      <c r="C13" s="45"/>
+      <c r="C13" s="40"/>
       <c r="G13" s="1">
         <v>11</v>
       </c>
@@ -6248,7 +8701,7 @@
         <f t="shared" ref="B14:B20" si="5">B13*(1+$M$31/100)</f>
         <v>43892807.494000003</v>
       </c>
-      <c r="C14" s="45" t="s">
+      <c r="C14" s="40" t="s">
         <v>111</v>
       </c>
       <c r="G14" s="1">
@@ -6301,7 +8754,7 @@
         <f t="shared" si="5"/>
         <v>44568756.729407609</v>
       </c>
-      <c r="C15" s="45"/>
+      <c r="C15" s="40"/>
       <c r="G15" s="1">
         <v>13</v>
       </c>
@@ -6352,7 +8805,7 @@
         <f t="shared" si="5"/>
         <v>45255115.583040491</v>
       </c>
-      <c r="C16" s="45"/>
+      <c r="C16" s="40"/>
       <c r="G16" s="1">
         <v>14</v>
       </c>
@@ -6403,7 +8856,7 @@
         <f t="shared" si="5"/>
         <v>45952044.363019317</v>
       </c>
-      <c r="C17" s="45"/>
+      <c r="C17" s="40"/>
       <c r="G17" s="1">
         <v>15</v>
       </c>
@@ -6454,7 +8907,7 @@
         <f t="shared" si="5"/>
         <v>46659705.846209817</v>
       </c>
-      <c r="C18" s="45"/>
+      <c r="C18" s="40"/>
       <c r="G18" s="1">
         <v>16</v>
       </c>
@@ -6505,7 +8958,7 @@
         <f t="shared" si="5"/>
         <v>47378265.316241451</v>
       </c>
-      <c r="C19" s="45"/>
+      <c r="C19" s="40"/>
       <c r="G19" s="1">
         <v>17</v>
       </c>
@@ -6556,7 +9009,7 @@
         <f t="shared" si="5"/>
         <v>48107890.602111571</v>
       </c>
-      <c r="C20" s="45"/>
+      <c r="C20" s="40"/>
       <c r="G20" s="1">
         <v>18</v>
       </c>
@@ -6607,11 +9060,11 @@
         <f>B20*(1+$N$31/100)</f>
         <v>48776590.281480923</v>
       </c>
-      <c r="C21" s="45"/>
-      <c r="G21" s="41" t="s">
+      <c r="C21" s="40"/>
+      <c r="G21" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="H21" s="41"/>
+      <c r="H21" s="43"/>
       <c r="I21" s="7"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
@@ -6639,7 +9092,7 @@
         <f>B21*(1+$N$31/100)</f>
         <v>49454584.88639351</v>
       </c>
-      <c r="C22" s="45"/>
+      <c r="C22" s="40"/>
       <c r="G22" s="1">
         <v>19</v>
       </c>
@@ -6690,7 +9143,7 @@
         <f>B22*(1+$N$31/100)</f>
         <v>50142003.616314381</v>
       </c>
-      <c r="C23" s="45"/>
+      <c r="C23" s="40"/>
       <c r="G23" s="1">
         <v>20</v>
       </c>
@@ -7036,10 +9489,10 @@
       </c>
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="G31" s="40" t="s">
+      <c r="G31" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="H31" s="40"/>
+      <c r="H31" s="42"/>
       <c r="I31" s="20">
         <v>43552.923000000003</v>
       </c>
@@ -7122,17 +9575,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="C4:C13"/>
-    <mergeCell ref="C14:C23"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="J1:L1"/>
     <mergeCell ref="G31:H31"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="G21:H21"/>
     <mergeCell ref="Q1:X1"/>
     <mergeCell ref="Y1:AA1"/>
     <mergeCell ref="M1:N1"/>
+    <mergeCell ref="C4:C13"/>
+    <mergeCell ref="C14:C23"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="J1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7154,7 +9607,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="40" t="s">
         <v>32</v>
       </c>
       <c r="B1" s="14" t="s">
@@ -7168,7 +9621,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="45"/>
+      <c r="A2" s="40"/>
       <c r="B2" s="14" t="s">
         <v>45</v>
       </c>
@@ -7449,7 +9902,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="40" t="s">
         <v>94</v>
       </c>
       <c r="B3" s="16">
@@ -7478,7 +9931,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="45"/>
+      <c r="A4" s="40"/>
       <c r="B4" s="16">
         <v>2001</v>
       </c>
@@ -7505,7 +9958,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="45"/>
+      <c r="A5" s="40"/>
       <c r="B5" s="16">
         <v>2002</v>
       </c>
@@ -7532,7 +9985,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="45"/>
+      <c r="A6" s="40"/>
       <c r="B6" s="16">
         <v>2003</v>
       </c>
@@ -7559,7 +10012,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="45"/>
+      <c r="A7" s="40"/>
       <c r="B7" s="16">
         <v>2004</v>
       </c>
@@ -7586,7 +10039,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="45"/>
+      <c r="A8" s="40"/>
       <c r="B8" s="16">
         <v>2005</v>
       </c>
@@ -7613,7 +10066,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="45"/>
+      <c r="A9" s="40"/>
       <c r="B9" s="16">
         <v>2006</v>
       </c>
@@ -7640,7 +10093,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="45"/>
+      <c r="A10" s="40"/>
       <c r="B10" s="16">
         <v>2007</v>
       </c>
@@ -7667,7 +10120,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="45"/>
+      <c r="A11" s="40"/>
       <c r="B11" s="16">
         <v>2008</v>
       </c>
@@ -7694,7 +10147,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="45"/>
+      <c r="A12" s="40"/>
       <c r="B12" s="16">
         <v>2009</v>
       </c>
@@ -7721,7 +10174,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="45"/>
+      <c r="A13" s="40"/>
       <c r="B13" s="16">
         <v>2010</v>
       </c>
@@ -7748,7 +10201,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="45"/>
+      <c r="A14" s="40"/>
       <c r="B14" s="16">
         <v>2011</v>
       </c>
@@ -7775,7 +10228,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="45"/>
+      <c r="A15" s="40"/>
       <c r="B15" s="16">
         <v>2012</v>
       </c>

</xml_diff>